<commit_message>
added one more row for user Hitesh
</commit_message>
<xml_diff>
--- a/Test_sheet1.xlsx
+++ b/Test_sheet1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>Connect</t>
+  </si>
+  <si>
+    <t>Hitesh</t>
+  </si>
+  <si>
+    <t>Compute</t>
   </si>
 </sst>
 </file>
@@ -392,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,6 +450,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>2121</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added business ops desc
</commit_message>
<xml_diff>
--- a/Test_sheet1.xlsx
+++ b/Test_sheet1.xlsx
@@ -46,7 +46,7 @@
     <t>Ashish</t>
   </si>
   <si>
-    <t>Ops</t>
+    <t>Business Ops</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
   <dimension ref="A2:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>